<commit_message>
review added in sound vendor
</commit_message>
<xml_diff>
--- a/back-end/Sound/VendorSignInData.xlsx
+++ b/back-end/Sound/VendorSignInData.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZone\wedding_planner\back-end\Garden\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86B884D-C0B6-40C2-B889-3C97B16C7C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10296"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>email</t>
   </si>
@@ -77,49 +71,13 @@
   </si>
   <si>
     <t>ling22313@yahoo.com</t>
-  </si>
-  <si>
-    <t>lotuseyecomputer@gmail.com</t>
-  </si>
-  <si>
-    <t>luckydeshwal.12@gmail.com</t>
-  </si>
-  <si>
-    <t>ravikant.gunjan@gmail.com</t>
-  </si>
-  <si>
-    <t>rhldxm@gmail.com</t>
-  </si>
-  <si>
-    <t>rinkukath0@gmail.com</t>
-  </si>
-  <si>
-    <t>rohitneema065@gmail.com</t>
-  </si>
-  <si>
-    <t>rshthakur80@gmail.com</t>
-  </si>
-  <si>
-    <t>safeercp073@gmail.com</t>
-  </si>
-  <si>
-    <t>sahilsharmanubgex@gmail.com</t>
-  </si>
-  <si>
-    <t>saikumar6448@gmail.com</t>
-  </si>
-  <si>
-    <t>saini.sourabh2013@gmail.com</t>
-  </si>
-  <si>
-    <t>santos_giannis@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -447,28 +405,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="6" max="6" width="83.7265625" customWidth="1"/>
-    <col min="7" max="7" width="36.26953125" customWidth="1"/>
-    <col min="11" max="11" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="83.77734375" customWidth="1"/>
+    <col min="7" max="7" width="36.21875" customWidth="1"/>
+    <col min="11" max="11" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -480,7 +438,7 @@
       <c r="F1" s="1"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -491,7 +449,7 @@
       <c r="F2" s="7"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
@@ -502,7 +460,7 @@
       <c r="F3" s="7"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -513,7 +471,7 @@
       <c r="F4" s="7"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -524,7 +482,7 @@
       <c r="F5" s="1"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
@@ -535,7 +493,7 @@
       <c r="F6" s="2"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
@@ -546,7 +504,7 @@
       <c r="F7" s="1"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
@@ -557,7 +515,7 @@
       <c r="F8" s="2"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
@@ -568,7 +526,7 @@
       <c r="F9" s="1"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
@@ -579,7 +537,7 @@
       <c r="F10" s="1"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
@@ -590,7 +548,7 @@
       <c r="F11" s="1"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -601,7 +559,7 @@
       <c r="F12" s="2"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
@@ -612,7 +570,7 @@
       <c r="F13" s="1"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>7</v>
       </c>
@@ -623,7 +581,7 @@
       <c r="F14" s="1"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
       <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
@@ -634,7 +592,7 @@
       <c r="F15" s="1"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>16</v>
       </c>
@@ -645,7 +603,7 @@
       <c r="F16" s="2"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
@@ -655,7 +613,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>18</v>
       </c>
@@ -665,1029 +623,969 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>123456</v>
-      </c>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A19" s="11"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <v>123456</v>
-      </c>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="11"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>123456</v>
-      </c>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" s="11"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <v>123456</v>
-      </c>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A22" s="11"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
-        <v>123456</v>
-      </c>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="11"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>123456</v>
-      </c>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" s="11"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25">
-        <v>123456</v>
-      </c>
+    <row r="25" spans="1:4" ht="14.4">
+      <c r="A25" s="11"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <v>123456</v>
-      </c>
+    <row r="26" spans="1:4" ht="14.4">
+      <c r="A26" s="11"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <v>123456</v>
-      </c>
+    <row r="27" spans="1:4" ht="14.4">
+      <c r="A27" s="11"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28">
-        <v>123456</v>
-      </c>
+    <row r="28" spans="1:4" ht="14.4">
+      <c r="A28" s="11"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>123456</v>
-      </c>
+    <row r="29" spans="1:4" ht="14.4">
+      <c r="A29" s="11"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>123456</v>
-      </c>
+    <row r="30" spans="1:4" ht="14.4">
+      <c r="A30" s="11"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="14.4">
       <c r="A31" s="12"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="14.4">
       <c r="A32" s="11"/>
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" ht="14.4">
       <c r="A33" s="12"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" ht="14.4">
       <c r="A34" s="11"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="14.4">
       <c r="A35" s="12"/>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="14.4">
       <c r="A36" s="11"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="14.4">
       <c r="A37" s="12"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="14.4">
       <c r="A38" s="11"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="14.4">
       <c r="A39" s="12"/>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="14.4">
       <c r="A40" s="11"/>
       <c r="B40" s="1"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="14.4">
       <c r="A41" s="12"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="14.4">
       <c r="A42" s="11"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" ht="14.4">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="14.4">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="14.4">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" ht="14.4">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="14.4">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="14.4">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="14.4">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="14.4">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="14.4">
       <c r="A51" s="2"/>
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" ht="14.4">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="14.4">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" ht="14.4">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="14.4">
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" ht="14.4">
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" ht="14.4">
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" ht="14.4">
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="14.4">
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" ht="14.4">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="14.4">
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="14.4">
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" ht="14.4">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="14.4">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:4" ht="14.4">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:4" ht="14.4">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:4" ht="14.4">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:4" ht="14.4">
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:4" ht="14.4">
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:4" ht="14.4">
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:4" ht="14.4">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:4" ht="14.4">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:4" ht="14.4">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:4" ht="14.4">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:4" ht="14.4">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:4" ht="14.4">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:4" ht="14.4">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:4" ht="14.4">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:4" ht="14.4">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:4" ht="14.4">
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:4" ht="14.4">
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:4" ht="14.4">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:4" ht="14.4">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:4" ht="14.4">
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:4" ht="14.4">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:4" ht="14.4">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:4" ht="14.4">
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:4" ht="14.4">
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:4" ht="14.4">
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:4" ht="14.4">
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:4" ht="14.4">
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:4" ht="14.4">
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:4" ht="14.4">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:4" ht="14.4">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:4" ht="14.4">
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:4" ht="14.4">
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:4" ht="14.4">
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:4" ht="14.4">
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:4" ht="14.4">
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:4" ht="14.4">
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:4" ht="14.4">
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:4" ht="14.4">
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:4" ht="14.4">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:4" ht="14.4">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:4" ht="14.4">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:4" ht="14.4">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:4" ht="14.4">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:4" ht="14.4">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:4" ht="14.4">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:4" ht="14.4">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:4" ht="14.4">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:4" ht="14.4">
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:4" ht="14.4">
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:4" ht="14.4">
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:4" ht="14.4">
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:4" ht="14.4">
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:4" ht="14.4">
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:4" ht="14.4">
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:4" ht="14.4">
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:4" ht="14.4">
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:4" ht="14.4">
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:4" ht="14.4">
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:4" ht="14.4">
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:4" ht="14.4">
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:4" ht="14.4">
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:4" ht="14.4">
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:4" ht="14.4">
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:4" ht="14.4">
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:4" ht="14.4">
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:4" ht="14.4">
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:4" ht="14.4">
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:4" ht="14.4">
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:4" ht="14.4">
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:4" ht="14.4">
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:4" ht="14.4">
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:4" ht="14.4">
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:4" ht="14.4">
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:4" ht="14.4">
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:4" ht="14.4">
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:4" ht="14.4">
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:4" ht="14.4">
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:4" ht="14.4">
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:4" ht="14.4">
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:4" ht="14.4">
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:4" ht="14.4">
       <c r="D145" s="1"/>
     </row>
-    <row r="146" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:4" ht="14.4">
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:4" ht="14.4">
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:4" ht="14.4">
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:4" ht="14.4">
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:4" ht="14.4">
       <c r="D150" s="2"/>
     </row>
-    <row r="151" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:4" ht="14.4">
       <c r="D151" s="2"/>
     </row>
-    <row r="152" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:4" ht="14.4">
       <c r="D152" s="2"/>
     </row>
-    <row r="153" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:4" ht="14.4">
       <c r="D153" s="2"/>
     </row>
-    <row r="154" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:4" ht="14.4">
       <c r="D154" s="2"/>
     </row>
-    <row r="155" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:4" ht="14.4">
       <c r="D155" s="2"/>
     </row>
-    <row r="156" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:4" ht="14.4">
       <c r="D156" s="2"/>
     </row>
-    <row r="157" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:4" ht="14.4">
       <c r="D157" s="2"/>
     </row>
-    <row r="158" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:4" ht="14.4">
       <c r="D158" s="2"/>
     </row>
-    <row r="159" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:4" ht="14.4">
       <c r="D159" s="2"/>
     </row>
-    <row r="160" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:4" ht="14.4">
       <c r="D160" s="2"/>
     </row>
-    <row r="161" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="4:4" ht="14.4">
       <c r="D161" s="2"/>
     </row>
-    <row r="162" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="4:4" ht="14.4">
       <c r="D162" s="2"/>
     </row>
-    <row r="163" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="4:4" ht="14.4">
       <c r="D163" s="2"/>
     </row>
-    <row r="164" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:4" ht="14.4">
       <c r="D164" s="2"/>
     </row>
-    <row r="165" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:4" ht="14.4">
       <c r="D165" s="2"/>
     </row>
-    <row r="166" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:4" ht="14.4">
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:4" ht="14.4">
       <c r="D167" s="2"/>
     </row>
-    <row r="168" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:4" ht="14.4">
       <c r="D168" s="2"/>
     </row>
-    <row r="169" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:4" ht="14.4">
       <c r="D169" s="2"/>
     </row>
-    <row r="170" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="4:4" ht="14.4">
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:4" ht="14.4">
       <c r="D171" s="2"/>
     </row>
-    <row r="172" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:4" ht="14.4">
       <c r="D172" s="2"/>
     </row>
-    <row r="173" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:4" ht="14.4">
       <c r="D173" s="2"/>
     </row>
-    <row r="174" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:4" ht="14.4">
       <c r="D174" s="2"/>
     </row>
-    <row r="175" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:4" ht="14.4">
       <c r="D175" s="2"/>
     </row>
-    <row r="176" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:4" ht="14.4">
       <c r="D176" s="2"/>
     </row>
-    <row r="177" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:4" ht="14.4">
       <c r="D177" s="2"/>
     </row>
-    <row r="178" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="4:4" ht="14.4">
       <c r="D178" s="2"/>
     </row>
-    <row r="179" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="4:4" ht="14.4">
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="4:4" ht="14.4">
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="4:4" ht="14.4">
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="4:4" ht="14.4">
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="4:4" ht="14.4">
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="4:4" ht="14.4">
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="4:4" ht="14.4">
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="4:4" ht="14.4">
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="4:4" ht="14.4">
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="4:4" ht="14.4">
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="4:4" ht="14.4">
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="4:4" ht="14.4">
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="4:4" ht="14.4">
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="4:4" ht="14.4">
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="4:4" ht="14.4">
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="4:4" ht="14.4">
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="4:4" ht="14.4">
       <c r="D195" s="1"/>
     </row>
-    <row r="196" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="4:4" ht="14.4">
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="4:4" ht="14.4">
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="4:4" ht="14.4">
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="4:4" ht="14.4">
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="4:4" ht="14.4">
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="201" spans="4:4" ht="14.4">
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="4:4" ht="14.4">
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="4:4" ht="14.4">
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="4:4" ht="14.4">
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="4:4" ht="14.4">
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="4:4" ht="14.4">
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="207" spans="4:4" ht="14.4">
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="4:4" ht="14.4">
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:4" ht="14.4">
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:4" ht="14.4">
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:4" ht="14.4">
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:4" ht="14.4">
       <c r="D212" s="2"/>
     </row>
-    <row r="213" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:4" ht="14.4">
       <c r="D213" s="2"/>
     </row>
-    <row r="214" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:4" ht="14.4">
       <c r="D214" s="2"/>
     </row>
-    <row r="215" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:4" ht="14.4">
       <c r="D215" s="2"/>
     </row>
-    <row r="216" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:4" ht="14.4">
       <c r="D216" s="2"/>
     </row>
-    <row r="217" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:4" ht="14.4">
       <c r="D217" s="2"/>
     </row>
-    <row r="218" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="4:4" ht="14.4">
       <c r="D218" s="2"/>
     </row>
-    <row r="219" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="219" spans="4:4" ht="14.4">
       <c r="D219" s="2"/>
     </row>
-    <row r="220" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="220" spans="4:4" ht="14.4">
       <c r="D220" s="1"/>
     </row>
-    <row r="221" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:4" ht="14.4">
       <c r="D221" s="2"/>
     </row>
-    <row r="222" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:4" ht="14.4">
       <c r="D222" s="2"/>
     </row>
-    <row r="223" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="4:4" ht="14.4">
       <c r="D223" s="2"/>
     </row>
-    <row r="224" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="4:4" ht="14.4">
       <c r="D224" s="2"/>
     </row>
-    <row r="225" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="4:4" ht="14.4">
       <c r="D225" s="2"/>
     </row>
-    <row r="226" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="4:4" ht="14.4">
       <c r="D226" s="2"/>
     </row>
-    <row r="227" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="4:4" ht="14.4">
       <c r="D227" s="2"/>
     </row>
-    <row r="228" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="4:4" ht="14.4">
       <c r="D228" s="2"/>
     </row>
-    <row r="229" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="4:4" ht="14.4">
       <c r="D229" s="2"/>
     </row>
-    <row r="230" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="230" spans="4:4" ht="14.4">
       <c r="D230" s="2"/>
     </row>
-    <row r="231" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="4:4" ht="14.4">
       <c r="D231" s="2"/>
     </row>
-    <row r="232" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="4:4" ht="14.4">
       <c r="D232" s="2"/>
     </row>
-    <row r="233" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="233" spans="4:4" ht="14.4">
       <c r="D233" s="2"/>
     </row>
-    <row r="234" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="234" spans="4:4" ht="14.4">
       <c r="D234" s="2"/>
     </row>
-    <row r="235" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="4:4" ht="14.4">
       <c r="D235" s="2"/>
     </row>
-    <row r="236" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="236" spans="4:4" ht="14.4">
       <c r="D236" s="2"/>
     </row>
-    <row r="237" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="4:4" ht="14.4">
       <c r="D237" s="2"/>
     </row>
-    <row r="238" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="238" spans="4:4" ht="14.4">
       <c r="D238" s="2"/>
     </row>
-    <row r="239" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="4:4" ht="14.4">
       <c r="D239" s="2"/>
     </row>
-    <row r="240" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="4:4" ht="14.4">
       <c r="D240" s="2"/>
     </row>
-    <row r="241" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="4:4" ht="14.4">
       <c r="D241" s="2"/>
     </row>
-    <row r="242" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="242" spans="4:4" ht="14.4">
       <c r="D242" s="2"/>
     </row>
-    <row r="243" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="243" spans="4:4" ht="14.4">
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="244" spans="4:4" ht="14.4">
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="245" spans="4:4" ht="14.4">
       <c r="D245" s="1"/>
     </row>
-    <row r="246" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="4:4" ht="14.4">
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="4:4" ht="14.4">
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="248" spans="4:4" ht="14.4">
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="249" spans="4:4" ht="14.4">
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="250" spans="4:4" ht="14.4">
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="251" spans="4:4" ht="14.4">
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="252" spans="4:4" ht="14.4">
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="253" spans="4:4" ht="14.4">
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="254" spans="4:4" ht="14.4">
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="4:4" ht="14.4">
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="256" spans="4:4" ht="14.4">
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="4:4" ht="14.4">
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="258" spans="4:4" ht="14.4">
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="259" spans="4:4" ht="14.4">
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="4:4" ht="14.4">
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="261" spans="4:4" ht="14.4">
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="262" spans="4:4" ht="14.4">
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="263" spans="4:4" ht="14.4">
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="264" spans="4:4" ht="14.4">
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="265" spans="4:4" ht="14.4">
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="266" spans="4:4" ht="14.4">
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="267" spans="4:4" ht="14.4">
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="268" spans="4:4" ht="14.4">
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="269" spans="4:4" ht="14.4">
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="270" spans="4:4" ht="14.4">
       <c r="D270" s="1"/>
     </row>
-    <row r="271" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="271" spans="4:4" ht="14.4">
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="272" spans="4:4" ht="14.4">
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="273" spans="4:4" ht="14.4">
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="274" spans="4:4" ht="14.4">
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="275" spans="4:4" ht="14.4">
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="276" spans="4:4" ht="14.4">
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="277" spans="4:4" ht="14.4">
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="278" spans="4:4" ht="14.4">
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="279" spans="4:4" ht="14.4">
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="280" spans="4:4" ht="14.4">
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="281" spans="4:4" ht="14.4">
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="282" spans="4:4" ht="14.4">
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="283" spans="4:4" ht="14.4">
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="284" spans="4:4" ht="14.4">
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="285" spans="4:4" ht="14.4">
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="286" spans="4:4" ht="14.4">
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="287" spans="4:4" ht="14.4">
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="288" spans="4:4" ht="14.4">
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="289" spans="4:4" ht="14.4">
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="290" spans="4:4" ht="14.4">
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="291" spans="4:4" ht="14.4">
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="292" spans="4:4" ht="14.4">
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="293" spans="4:4" ht="14.4">
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="294" spans="4:4" ht="14.4">
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="4:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="295" spans="4:4" ht="14.4">
       <c r="D295" s="1"/>
     </row>
-    <row r="296" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="296" spans="4:4" ht="14.4">
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="297" spans="4:4" ht="14.4">
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="298" spans="4:4" ht="14.4">
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="299" spans="4:4" ht="14.4">
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="300" spans="4:4" ht="14.4">
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="301" spans="4:4" ht="14.4">
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="302" spans="4:4" ht="14.4">
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="303" spans="4:4" ht="14.4">
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="304" spans="4:4" ht="14.4">
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="305" spans="4:4" ht="14.4">
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="306" spans="4:4" ht="14.4">
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="4:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="307" spans="4:4" ht="14.4">
       <c r="D307" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{376BE002-049A-4626-AB16-48E8CEE0C3BB}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{689A2E0B-2B00-42C6-A215-57D8679DBD4F}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{445745BA-38F3-4121-818F-114F48EC19D1}"/>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>